<commit_message>
array practice questions implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestDataSheet.xlsx
+++ b/src/test/resources/TestData/TestDataSheet.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5618DA00-8B36-4B95-BB58-40D2798BBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5230324B-6DE3-4594-818B-02633532C9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
     <sheet name="pythonCode" sheetId="2" r:id="rId2"/>
-    <sheet name="Practice Qns" sheetId="3" r:id="rId3"/>
+    <sheet name="Practice Questions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Vijayabharathi</t>
   </si>
@@ -68,12 +68,6 @@
 \b
 \b
 search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>Element Found</t>
-  </si>
-  <si>
-    <t>submission success</t>
   </si>
   <si>
     <t>def findMaxConsecutiveOnes(nums) :
@@ -95,9 +89,6 @@
 \b
 \b
 findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>def findNumbers(nums):
@@ -129,9 +120,6 @@
 sortedSquares([-7,-3,2,3,11])</t>
   </si>
   <si>
-    <t>[4, 9, 9, 49, 121]</t>
-  </si>
-  <si>
     <t>TC002</t>
   </si>
   <si>
@@ -141,17 +129,14 @@
     <t>print("hello")</t>
   </si>
   <si>
-    <t>print("Hello")</t>
-  </si>
-  <si>
-    <t>TestId</t>
+    <t>NameError: name 'hello' is not defined on line 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -182,6 +167,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -210,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -220,6 +211,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,20 +581,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157208-34A5-4823-827D-AB44E091375F}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
+      <c r="A1" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
@@ -612,70 +603,52 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="C11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -684,85 +657,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2F416-0080-4CD5-8640-78BD573AE583}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed array feature run issues
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestDataSheet.xlsx
+++ b/src/test/resources/TestData/TestDataSheet.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5230324B-6DE3-4594-818B-02633532C9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\god\eclipse-workspace\DS-AlgoProj\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8726EDC4-9EE6-4A66-887B-6D65BCF411A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="251" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="371" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginSheet" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,11 @@
     <sheet name="Practice Questions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Vijayabharathi</t>
   </si>
@@ -579,76 +583,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08157208-34A5-4823-827D-AB44E091375F}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="243.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="243.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -659,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB2F416-0080-4CD5-8640-78BD573AE583}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>